<commit_message>
CoffinLastCreate, FireDragonLastCreate 어펙터밸류 추가 CoffinLastSkillInfo, FireDragonAreaSkillInfo 이펙트 어드레스 연결 그외 밸런싱 적힌 내용 수정
</commit_message>
<xml_diff>
--- a/Excel/Action.xlsx
+++ b/Excel/Action.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1D2072-5D3D-4335-BAE7-B396DCDADC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911EFA6D-DE56-4B6C-AB38-4E423105F4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{68A32D28-3263-434A-A46E-6AC4AEF62380}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="276">
   <si>
     <t>actorId|String</t>
   </si>
@@ -738,9 +738,6 @@
     <t>Spell_Coffin</t>
   </si>
   <si>
-    <t>CoffinSkillInfo</t>
-  </si>
-  <si>
     <t>Spell_FrozenMine</t>
   </si>
   <si>
@@ -762,9 +759,6 @@
     <t>TornadoCreate</t>
   </si>
   <si>
-    <t>CoffinCreate</t>
-  </si>
-  <si>
     <t>FrozenMineCreate</t>
   </si>
   <si>
@@ -777,12 +771,6 @@
     <t>Spell_FireDragon</t>
   </si>
   <si>
-    <t>FireDragonCreate</t>
-  </si>
-  <si>
-    <t>FireDragonSkillInfo</t>
-  </si>
-  <si>
     <t>Spell_BigSword</t>
   </si>
   <si>
@@ -862,6 +850,21 @@
   </si>
   <si>
     <t>45, 75</t>
+  </si>
+  <si>
+    <t>CoffinCreate, CoffinLastCreate</t>
+  </si>
+  <si>
+    <t>CoffinSkillInfo, CoffinLastSkillInfo</t>
+  </si>
+  <si>
+    <t>FireDragonCreate, FireDragonLastCreate</t>
+  </si>
+  <si>
+    <t>FireDragonSkillInfo, FireDragonAreaSkillInfo</t>
+  </si>
+  <si>
+    <t>1640, 30</t>
   </si>
 </sst>
 </file>
@@ -2940,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L13" t="s">
         <v>166</v>
@@ -2996,7 +2999,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L14" t="s">
         <v>162</v>
@@ -3052,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L15" t="s">
         <v>164</v>
@@ -3108,7 +3111,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="L16" t="s">
         <v>166</v>
@@ -3132,7 +3135,7 @@
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -3152,7 +3155,7 @@
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H17">
         <v>10</v>
@@ -3164,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L17" t="s">
         <v>162</v>
@@ -3188,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -3208,7 +3211,7 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -3220,7 +3223,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L18" t="s">
         <v>164</v>
@@ -3244,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -3317,7 +3320,7 @@
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H20">
         <v>10</v>
@@ -3329,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="L20" t="s">
         <v>162</v>
@@ -3353,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -3373,7 +3376,7 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -3385,7 +3388,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L21" t="s">
         <v>164</v>
@@ -3409,12 +3412,12 @@
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -3429,7 +3432,7 @@
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H22">
         <v>17</v>
@@ -3441,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="L22" t="s">
         <v>164</v>
@@ -3465,12 +3468,12 @@
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -3485,7 +3488,7 @@
         <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H23">
         <v>19</v>
@@ -3497,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="L23" t="s">
         <v>164</v>
@@ -3521,12 +3524,12 @@
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -3541,7 +3544,7 @@
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H24">
         <v>15</v>
@@ -3553,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L24" t="s">
         <v>164</v>
@@ -3577,12 +3580,12 @@
         <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -3597,7 +3600,7 @@
         <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H25">
         <v>20</v>
@@ -3609,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="L25" t="s">
         <v>164</v>
@@ -3633,12 +3636,12 @@
         <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -3653,7 +3656,7 @@
         <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H26">
         <v>30</v>
@@ -3665,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="L26" t="s">
         <v>164</v>
@@ -3689,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -3735,7 +3738,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -5119,7 +5122,7 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -5163,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -5185,7 +5188,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -5195,8 +5198,8 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="H30">
-        <v>1640</v>
+      <c r="H30" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -5212,7 +5215,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5223,40 +5226,40 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>820</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>120</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B36">
         <v>1</v>

</xml_diff>